<commit_message>
expand TAL and sorbate scenario analyses
</commit_message>
<xml_diff>
--- a/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
+++ b/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\biorefineries\TAL\analyses\full\parameter_distributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FFAD89-24CD-4861-ABF6-737C9834958A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB9BB05-CC73-486D-83CC-3D6590A0ACF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -828,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1293,22 +1293,22 @@
         <v>62</v>
       </c>
       <c r="E14" s="3">
-        <v>11901</v>
+        <v>15944</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G14" s="3">
         <f>0.8*E14</f>
-        <v>9520.8000000000011</v>
+        <v>12755.2</v>
       </c>
       <c r="H14" s="3">
         <f>E14</f>
-        <v>11901</v>
+        <v>15944</v>
       </c>
       <c r="I14" s="3">
         <f>1.2*E14</f>
-        <v>14281.199999999999</v>
+        <v>19132.8</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3" t="s">

</xml_diff>

<commit_message>
update catalytic upgrading parameter distributions
</commit_message>
<xml_diff>
--- a/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
+++ b/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\biorefineries\TAL\analyses\full\parameter_distributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB9BB05-CC73-486D-83CC-3D6590A0ACF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3AA316-221A-4B21-B330-43870AB2AEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -828,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2176,13 +2176,13 @@
         <v>22</v>
       </c>
       <c r="G41" s="3">
-        <f>0.8*E41</f>
-        <v>4.88</v>
+        <f>0.9*E41</f>
+        <v>5.49</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="3">
-        <f>1.2*E41</f>
-        <v>7.3199999999999994</v>
+        <f>1.1*E41</f>
+        <v>6.71</v>
       </c>
       <c r="J41" s="3"/>
       <c r="K41" s="3" t="s">
@@ -2209,13 +2209,13 @@
         <v>22</v>
       </c>
       <c r="G42" s="3">
-        <f>0.8*E42</f>
-        <v>128</v>
+        <f>0.9*E42</f>
+        <v>144</v>
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3">
-        <f>1.2*E42</f>
-        <v>192</v>
+        <f>1.1*E42</f>
+        <v>176</v>
       </c>
       <c r="J42" s="3"/>
       <c r="K42" s="3" t="s">

</xml_diff>

<commit_message>
update pH loading command in scenario analyses
</commit_message>
<xml_diff>
--- a/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
+++ b/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\biorefineries\TAL\analyses\full\parameter_distributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3AA316-221A-4B21-B330-43870AB2AEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD1BA61-35F5-447E-BB58-689D0DFD1C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -828,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K59" sqref="K59"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update IRR to 10% (8-12%)
</commit_message>
<xml_diff>
--- a/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
+++ b/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\biorefineries\TAL\analyses\full\parameter_distributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD1BA61-35F5-447E-BB58-689D0DFD1C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7583DC-D92F-45E9-9788-C864851CE911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -829,7 +829,7 @@
   <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1360,17 +1360,17 @@
         <v>8</v>
       </c>
       <c r="E16" s="3">
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G16" s="3">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3" t="s">

</xml_diff>

<commit_message>
update baseline and improved reaction times and add SA_THF_Ethanol system and scenario
</commit_message>
<xml_diff>
--- a/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
+++ b/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\biorefineries\TAL\analyses\full\parameter_distributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CC46AC-BFF2-457F-B1F6-216B8913534A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5438C72-20DF-41C7-80B4-7383D8BD445A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="145">
   <si>
     <t>Parameter name</t>
   </si>
@@ -323,12 +323,6 @@
     <t>R302.air_flow_rate_safety_factor_for_DO_saturation_basis = x</t>
   </si>
   <si>
-    <t>Acetone unit price</t>
-  </si>
-  <si>
-    <t>acetone_fresh.price = x</t>
-  </si>
-  <si>
     <t>Ni-SiO2 catalyst unit price</t>
   </si>
   <si>
@@ -459,6 +453,24 @@
   </si>
   <si>
     <t>R403.P = x</t>
+  </si>
+  <si>
+    <t>M405.w_IPA_per_w_TAL = x</t>
+  </si>
+  <si>
+    <t>M406.w_IPA_per_w_KSA = x</t>
+  </si>
+  <si>
+    <t>kg-IPA/kg-TAL</t>
+  </si>
+  <si>
+    <t>Upgrading IPA:TAL mass ratio</t>
+  </si>
+  <si>
+    <t>Purification IPA:KS mass ratio</t>
+  </si>
+  <si>
+    <t>kg-IPA/kg-KS</t>
   </si>
 </sst>
 </file>
@@ -819,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1138,7 +1150,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>7</v>
@@ -1150,28 +1162,26 @@
         <v>10</v>
       </c>
       <c r="E10" s="3">
-        <v>1.5629</v>
+        <v>1.069</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="3">
-        <f>1.5629*0.44/0.63</f>
-        <v>1.0915492063492063</v>
+        <v>0.99399999999999999</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3">
-        <f>1.5629*0.82/0.63</f>
-        <v>2.0342507936507936</v>
+        <v>1.2809999999999999</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>7</v>
@@ -1183,26 +1193,29 @@
         <v>10</v>
       </c>
       <c r="E11" s="3">
-        <v>1.069</v>
+        <v>33</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="G11" s="3">
-        <v>0.99399999999999999</v>
-      </c>
-      <c r="H11" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="H11" s="3">
+        <f t="shared" ref="H11" si="0">E11</f>
+        <v>33</v>
+      </c>
       <c r="I11" s="3">
-        <v>1.2809999999999999</v>
+        <v>50</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>7</v>
@@ -1214,98 +1227,95 @@
         <v>10</v>
       </c>
       <c r="E12" s="3">
-        <v>33</v>
+        <v>1.4419999999999999</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G12" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" ref="H12:H13" si="0">E12</f>
-        <v>33</v>
+        <v>1.4419999999999999</v>
       </c>
       <c r="I12" s="3">
-        <v>50</v>
+        <v>2.1</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="E13" s="3">
-        <v>1.4419999999999999</v>
+        <v>15944</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="3">
-        <v>1</v>
+        <f>0.8*E13</f>
+        <v>12755.2</v>
       </c>
       <c r="H13" s="3">
-        <v>1.4419999999999999</v>
+        <f>E13</f>
+        <v>15944</v>
       </c>
       <c r="I13" s="3">
-        <v>2.1</v>
+        <f>1.2*E13</f>
+        <v>19132.8</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3" t="s">
-        <v>133</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="E14" s="3">
-        <v>15944</v>
+        <v>0.21</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="G14" s="3">
-        <f>0.8*E14</f>
-        <v>12755.2</v>
-      </c>
-      <c r="H14" s="3">
-        <f>E14</f>
-        <v>15944</v>
-      </c>
+        <v>0.15</v>
+      </c>
+      <c r="H14" s="3"/>
       <c r="I14" s="3">
-        <f>1.2*E14</f>
-        <v>19132.8</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>7</v>
@@ -1317,57 +1327,59 @@
         <v>8</v>
       </c>
       <c r="E15" s="3">
-        <v>0.21</v>
+        <v>0.1</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G15" s="3">
-        <v>0.15</v>
+        <v>0.08</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3">
-        <v>0.28000000000000003</v>
+        <v>0.12</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E16" s="3">
-        <v>0.1</v>
+        <v>76.903000000000006</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G16" s="3">
-        <v>0.08</v>
+        <v>41.707000000000001</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3">
-        <v>0.12</v>
-      </c>
-      <c r="J16" s="3"/>
+        <v>101.9</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="K16" s="3" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>45</v>
@@ -1379,28 +1391,28 @@
         <v>12</v>
       </c>
       <c r="E17" s="3">
-        <v>76.903000000000006</v>
+        <v>10.228</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G17" s="3">
-        <v>41.707000000000001</v>
+        <v>5.5469999999999997</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3">
-        <v>101.9</v>
+        <v>14.909000000000001</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>77</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>45</v>
@@ -1409,31 +1421,31 @@
         <v>27</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="E18" s="3">
-        <v>10.228</v>
+        <v>10</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G18" s="3">
-        <v>5.5469999999999997</v>
+        <f>0.8*E18</f>
+        <v>8</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3">
-        <v>14.909000000000001</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>77</v>
-      </c>
+        <f>1.2*E18</f>
+        <v>12</v>
+      </c>
+      <c r="J18" s="5"/>
       <c r="K18" s="3" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>45</v>
@@ -1442,31 +1454,29 @@
         <v>27</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>92</v>
+        <v>8</v>
       </c>
       <c r="E19" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G19" s="3">
-        <f>0.8*E19</f>
-        <v>8</v>
+        <v>0.5</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3">
-        <f>1.2*E19</f>
-        <v>12</v>
-      </c>
-      <c r="J19" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="J19" s="3"/>
       <c r="K19" s="3" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>93</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>45</v>
@@ -1478,26 +1488,27 @@
         <v>8</v>
       </c>
       <c r="E20" s="3">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G20" s="3">
-        <v>0.5</v>
+        <f>0.9*E20</f>
+        <v>0.85499999999999998</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>45</v>
@@ -1509,27 +1520,28 @@
         <v>8</v>
       </c>
       <c r="E21" s="3">
-        <v>0.95</v>
+        <v>0.05</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G21" s="3">
         <f>0.9*E21</f>
-        <v>0.85499999999999998</v>
+        <v>4.5000000000000005E-2</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3">
-        <v>1</v>
+        <f>1.1*E21</f>
+        <v>5.5000000000000007E-2</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>45</v>
@@ -1538,31 +1550,31 @@
         <v>27</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E22" s="3">
-        <v>0.05</v>
+        <v>0.40479999999999999</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G22" s="3">
-        <f>0.9*E22</f>
-        <v>4.5000000000000005E-2</v>
+        <f>0.8*E22</f>
+        <v>0.32384000000000002</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3">
-        <f>1.1*E22</f>
-        <v>5.5000000000000007E-2</v>
+        <f>1.2*E22</f>
+        <v>0.48575999999999997</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>45</v>
@@ -1571,31 +1583,31 @@
         <v>27</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E23" s="3">
-        <v>0.40479999999999999</v>
+        <v>35.9</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G23" s="3">
-        <f>0.8*E23</f>
-        <v>0.32384000000000002</v>
+        <f>E23*0.8</f>
+        <v>28.72</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3">
-        <f>1.2*E23</f>
-        <v>0.48575999999999997</v>
+        <f>E23*1.2</f>
+        <v>43.08</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>45</v>
@@ -1604,31 +1616,31 @@
         <v>27</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="3">
-        <v>35.9</v>
+        <v>30</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0.12</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G24" s="3">
         <f>E24*0.8</f>
-        <v>28.72</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3">
         <f>E24*1.2</f>
-        <v>43.08</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>45</v>
@@ -1637,31 +1649,31 @@
         <v>27</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="4">
-        <v>0.12</v>
+        <v>20</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.33900000000000002</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G25" s="3">
         <f>E25*0.8</f>
-        <v>9.6000000000000002E-2</v>
+        <v>0.27120000000000005</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3">
         <f>E25*1.2</f>
-        <v>0.14399999999999999</v>
+        <v>0.40679999999999999</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>45</v>
@@ -1673,31 +1685,31 @@
         <v>20</v>
       </c>
       <c r="E26" s="3">
-        <v>0.33900000000000002</v>
+        <v>8.856E-2</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G26" s="3">
         <f>E26*0.8</f>
-        <v>0.27120000000000005</v>
+        <v>7.0848000000000008E-2</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3">
         <f>E26*1.2</f>
-        <v>0.40679999999999999</v>
+        <v>0.10627199999999999</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>27</v>
@@ -1706,28 +1718,26 @@
         <v>20</v>
       </c>
       <c r="E27" s="3">
-        <v>8.856E-2</v>
+        <v>0.2087</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G27" s="3">
-        <f>E27*0.8</f>
-        <v>7.0848000000000008E-2</v>
+        <v>4.6300000000000001E-2</v>
       </c>
       <c r="H27" s="3"/>
-      <c r="I27" s="3">
-        <f>E27*1.2</f>
-        <v>0.10627199999999999</v>
+      <c r="I27" s="4">
+        <v>0.34</v>
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>55</v>
@@ -1736,29 +1746,29 @@
         <v>27</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E28" s="3">
-        <v>0.2087</v>
+        <v>1</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G28" s="3">
-        <v>4.6300000000000001E-2</v>
+        <v>0.8</v>
       </c>
       <c r="H28" s="3"/>
-      <c r="I28" s="4">
-        <v>0.34</v>
+      <c r="I28" s="3">
+        <v>1.2</v>
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="3" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>55</v>
@@ -1767,29 +1777,29 @@
         <v>27</v>
       </c>
       <c r="D29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="3">
         <v>8</v>
       </c>
-      <c r="E29" s="3">
-        <v>1</v>
-      </c>
       <c r="F29" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G29" s="3">
-        <v>0.8</v>
+        <v>2</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3">
-        <v>1.2</v>
+        <v>14</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>55</v>
@@ -1798,29 +1808,30 @@
         <v>27</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E30" s="3">
-        <v>8</v>
+        <v>0.95</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G30" s="3">
-        <v>2</v>
+        <f>E30*0.8</f>
+        <v>0.76</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="3" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>55</v>
@@ -1832,27 +1843,28 @@
         <v>8</v>
       </c>
       <c r="E31" s="3">
-        <v>0.95</v>
+        <v>0.5</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G31" s="3">
         <f>E31*0.8</f>
-        <v>0.76</v>
+        <v>0.4</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3">
-        <v>1</v>
+        <f>E31*1.2</f>
+        <v>0.6</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>55</v>
@@ -1864,85 +1876,85 @@
         <v>8</v>
       </c>
       <c r="E32" s="3">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G32" s="3">
         <f>E32*0.8</f>
-        <v>0.4</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3">
         <f>E32*1.2</f>
-        <v>0.6</v>
+        <v>0.06</v>
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="E33" s="3">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G33" s="3">
-        <f>E33*0.8</f>
-        <v>4.0000000000000008E-2</v>
+        <f t="shared" ref="G33:G37" si="1">0.9*E33</f>
+        <v>0.18000000000000002</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3">
-        <f>E33*1.2</f>
-        <v>0.06</v>
+        <f>1.1*E33</f>
+        <v>0.22000000000000003</v>
       </c>
       <c r="J33" s="3"/>
       <c r="K33" s="3" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>102</v>
+        <v>15</v>
       </c>
       <c r="E34" s="3">
-        <v>0.2</v>
+        <v>1.9</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G34" s="3">
-        <f t="shared" ref="G34:G38" si="1">0.9*E34</f>
-        <v>0.18000000000000002</v>
+        <f t="shared" si="1"/>
+        <v>1.71</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3">
         <f>1.1*E34</f>
-        <v>0.22000000000000003</v>
+        <v>2.09</v>
       </c>
       <c r="J34" s="3"/>
       <c r="K34" s="3" t="s">
@@ -1954,190 +1966,190 @@
         <v>104</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>15</v>
+        <v>105</v>
       </c>
       <c r="E35" s="3">
-        <v>9.4</v>
+        <v>100</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G35" s="3">
         <f t="shared" si="1"/>
-        <v>8.4600000000000009</v>
+        <v>90</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3">
         <f>1.1*E35</f>
-        <v>10.340000000000002</v>
+        <v>110.00000000000001</v>
       </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E36" s="3">
-        <v>100</v>
+        <v>3500000</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G36" s="3">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>3150000</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3">
         <f>1.1*E36</f>
-        <v>110.00000000000001</v>
+        <v>3850000.0000000005</v>
       </c>
       <c r="J36" s="3"/>
       <c r="K36" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>110</v>
+        <v>8</v>
       </c>
       <c r="E37" s="3">
-        <v>3500000</v>
+        <v>0.96899999999999997</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G37" s="3">
         <f t="shared" si="1"/>
-        <v>3150000</v>
+        <v>0.87209999999999999</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="3">
-        <f>1.1*E37</f>
-        <v>3850000.0000000005</v>
+        <v>1</v>
       </c>
       <c r="J37" s="3"/>
       <c r="K37" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="E38" s="3">
-        <v>0.96899999999999997</v>
+        <v>1</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G38" s="3">
-        <f t="shared" si="1"/>
-        <v>0.87209999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="3">
-        <v>1</v>
+        <v>1.9</v>
       </c>
       <c r="J38" s="3"/>
       <c r="K38" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E39" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G39" s="3">
-        <v>0.1</v>
+        <f>0.9*E39</f>
+        <v>0.45</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="3">
-        <v>1.9</v>
+        <f>1.1*E39</f>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J39" s="3"/>
       <c r="K39" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>102</v>
+        <v>15</v>
       </c>
       <c r="E40" s="3">
-        <v>0.5</v>
+        <v>3.1</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G40" s="3">
         <f>0.9*E40</f>
-        <v>0.45</v>
+        <v>2.79</v>
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="3">
         <f>1.1*E40</f>
-        <v>0.55000000000000004</v>
+        <v>3.4100000000000006</v>
       </c>
       <c r="J40" s="3"/>
       <c r="K40" s="3" t="s">
@@ -2149,28 +2161,28 @@
         <v>117</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>15</v>
+        <v>105</v>
       </c>
       <c r="E41" s="3">
-        <v>6.1</v>
+        <v>160</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G41" s="3">
         <f>0.9*E41</f>
-        <v>5.49</v>
+        <v>144</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="3">
         <f>1.1*E41</f>
-        <v>6.71</v>
+        <v>176</v>
       </c>
       <c r="J41" s="3"/>
       <c r="K41" s="3" t="s">
@@ -2182,28 +2194,28 @@
         <v>119</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
       <c r="E42" s="3">
-        <v>160</v>
+        <v>0.871</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G42" s="3">
         <f>0.9*E42</f>
-        <v>144</v>
+        <v>0.78390000000000004</v>
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3">
         <f>1.1*E42</f>
-        <v>176</v>
+        <v>0.95810000000000006</v>
       </c>
       <c r="J42" s="3"/>
       <c r="K42" s="3" t="s">
@@ -2215,28 +2227,28 @@
         <v>121</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="E43" s="3">
-        <v>0.871</v>
+        <v>2000000</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G43" s="3">
         <f>0.9*E43</f>
-        <v>0.78390000000000004</v>
+        <v>1800000</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="3">
         <f>1.1*E43</f>
-        <v>0.95810000000000006</v>
+        <v>2200000</v>
       </c>
       <c r="J43" s="3"/>
       <c r="K43" s="3" t="s">
@@ -2248,28 +2260,26 @@
         <v>123</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E44" s="3">
-        <v>2000000</v>
+        <v>1</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G44" s="3">
-        <f>0.9*E44</f>
-        <v>1800000</v>
+        <v>0.1</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="3">
-        <f>1.1*E44</f>
-        <v>2200000</v>
+        <v>1.9</v>
       </c>
       <c r="J44" s="3"/>
       <c r="K44" s="3" t="s">
@@ -2281,26 +2291,28 @@
         <v>125</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>114</v>
+        <v>15</v>
       </c>
       <c r="E45" s="3">
-        <v>1</v>
+        <v>9.51</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G45" s="3">
-        <v>0.1</v>
+        <f>0.9*E45</f>
+        <v>8.5589999999999993</v>
       </c>
       <c r="H45" s="3"/>
       <c r="I45" s="3">
-        <v>1.9</v>
+        <f>1.1*E45</f>
+        <v>10.461</v>
       </c>
       <c r="J45" s="3"/>
       <c r="K45" s="3" t="s">
@@ -2309,62 +2321,63 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E46" s="3">
-        <v>19</v>
+        <v>0.999</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G46" s="3">
-        <f>0.9*E46</f>
-        <v>17.100000000000001</v>
+        <v>0.98</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="3">
-        <f>1.1*E46</f>
-        <v>20.900000000000002</v>
+        <v>1</v>
       </c>
       <c r="J46" s="3"/>
       <c r="K46" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>8</v>
+        <v>105</v>
       </c>
       <c r="E47" s="3">
-        <v>0.999</v>
+        <f>130</f>
+        <v>130</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G47" s="3">
-        <v>0.98</v>
+        <f>0.9*E47</f>
+        <v>117</v>
       </c>
       <c r="H47" s="3"/>
       <c r="I47" s="3">
-        <v>1</v>
+        <f>1.1*E47</f>
+        <v>143</v>
       </c>
       <c r="J47" s="3"/>
       <c r="K47" s="3" t="s">
@@ -2373,140 +2386,135 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E48" s="3">
-        <f>130</f>
-        <v>130</v>
+        <v>2000000</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G48" s="3">
         <f>0.9*E48</f>
-        <v>117</v>
+        <v>1800000</v>
       </c>
       <c r="H48" s="3"/>
       <c r="I48" s="3">
         <f>1.1*E48</f>
-        <v>143</v>
+        <v>2200000</v>
       </c>
       <c r="J48" s="3"/>
       <c r="K48" s="3" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>27</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="E49" s="3">
-        <v>2000000</v>
+        <v>31.391999999999999</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G49" s="3">
-        <f>0.9*E49</f>
-        <v>1800000</v>
+        <f t="shared" ref="G49:G50" si="2">0.9*E49</f>
+        <v>28.252800000000001</v>
       </c>
       <c r="H49" s="3"/>
       <c r="I49" s="3">
-        <f>1.1*E49</f>
-        <v>2200000</v>
+        <f t="shared" ref="I49:I50" si="3">1.1*E49</f>
+        <v>34.531200000000005</v>
       </c>
       <c r="J49" s="3"/>
       <c r="K49" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>27</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>15</v>
+        <v>144</v>
       </c>
       <c r="E50" s="3">
-        <v>168</v>
+        <v>31.545000000000002</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="G50" s="3">
-        <v>134.4</v>
-      </c>
-      <c r="H50" s="3">
-        <v>168</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>28.390500000000003</v>
+      </c>
+      <c r="H50" s="3"/>
       <c r="I50" s="3">
-        <v>201.6</v>
+        <f t="shared" si="3"/>
+        <v>34.699500000000008</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="3" t="s">
-        <v>63</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>24</v>
+        <v>136</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E51" s="3">
-        <v>0.8</v>
+        <v>168</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="G51" s="3">
-        <f>E51*0.9</f>
-        <v>0.72000000000000008</v>
-      </c>
-      <c r="H51" s="3"/>
+        <v>134.4</v>
+      </c>
+      <c r="H51" s="3">
+        <v>168</v>
+      </c>
       <c r="I51" s="3">
-        <f>E51*1.1</f>
-        <v>0.88000000000000012</v>
+        <v>201.6</v>
       </c>
       <c r="J51" s="3"/>
       <c r="K51" s="3" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>23</v>
@@ -2518,22 +2526,55 @@
         <v>8</v>
       </c>
       <c r="E52" s="3">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G52" s="3">
         <f>E52*0.9</f>
-        <v>0.76500000000000001</v>
+        <v>0.72000000000000008</v>
       </c>
       <c r="H52" s="3"/>
       <c r="I52" s="3">
         <f>E52*1.1</f>
-        <v>0.93500000000000005</v>
+        <v>0.88000000000000012</v>
       </c>
       <c r="J52" s="3"/>
       <c r="K52" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53" s="3">
+        <f>E53*0.9</f>
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3">
+        <f>E53*1.1</f>
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update hydrogenation and improved dehydration conv ranges
</commit_message>
<xml_diff>
--- a/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
+++ b/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\biorefineries\TAL\analyses\full\parameter_distributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5438C72-20DF-41C7-80B4-7383D8BD445A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{734497CB-6070-42A1-B021-9C8F66FDC84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -831,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -847,7 +847,7 @@
     <col min="11" max="11" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -882,7 +882,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
@@ -912,8 +912,12 @@
       <c r="K2" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q2">
+        <f>IF(E2=H2, 1, IF(F2=$F$2, 1, 0))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>78</v>
       </c>
@@ -948,8 +952,12 @@
       <c r="K3" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q53" si="0">IF(E3=H3, 1, IF(F3=$F$2, 1, 0))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -981,8 +989,12 @@
       <c r="K4" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -1014,8 +1026,12 @@
       <c r="K5" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1047,8 +1063,12 @@
       <c r="K6" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
@@ -1083,8 +1103,12 @@
       <c r="K7" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>51</v>
       </c>
@@ -1116,8 +1140,12 @@
       <c r="K8" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>90</v>
       </c>
@@ -1147,8 +1175,12 @@
       <c r="K9" s="3" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>97</v>
       </c>
@@ -1178,8 +1210,12 @@
       <c r="K10" s="3" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>95</v>
       </c>
@@ -1202,7 +1238,7 @@
         <v>5</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" ref="H11" si="0">E11</f>
+        <f t="shared" ref="H11" si="1">E11</f>
         <v>33</v>
       </c>
       <c r="I11" s="3">
@@ -1212,8 +1248,12 @@
       <c r="K11" s="3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>96</v>
       </c>
@@ -1245,8 +1285,12 @@
       <c r="K12" s="3" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>61</v>
       </c>
@@ -1281,8 +1325,12 @@
       <c r="K13" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>81</v>
       </c>
@@ -1312,8 +1360,12 @@
       <c r="K14" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>82</v>
       </c>
@@ -1343,8 +1395,12 @@
       <c r="K15" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
@@ -1376,8 +1432,12 @@
       <c r="K16" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>88</v>
       </c>
@@ -1409,8 +1469,12 @@
       <c r="K17" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>43</v>
       </c>
@@ -1442,8 +1506,12 @@
       <c r="K18" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>93</v>
       </c>
@@ -1473,8 +1541,12 @@
       <c r="K19" s="3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -1505,8 +1577,12 @@
       <c r="K20" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>40</v>
       </c>
@@ -1538,8 +1614,12 @@
       <c r="K21" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>47</v>
       </c>
@@ -1571,8 +1651,12 @@
       <c r="K22" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>48</v>
       </c>
@@ -1604,8 +1688,12 @@
       <c r="K23" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>49</v>
       </c>
@@ -1637,8 +1725,12 @@
       <c r="K24" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>74</v>
       </c>
@@ -1670,8 +1762,12 @@
       <c r="K25" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>72</v>
       </c>
@@ -1703,8 +1799,12 @@
       <c r="K26" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>70</v>
       </c>
@@ -1734,8 +1834,12 @@
       <c r="K27" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>86</v>
       </c>
@@ -1765,8 +1869,12 @@
       <c r="K28" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>54</v>
       </c>
@@ -1796,8 +1904,12 @@
       <c r="K29" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>65</v>
       </c>
@@ -1828,8 +1940,12 @@
       <c r="K30" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>66</v>
       </c>
@@ -1861,8 +1977,12 @@
       <c r="K31" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>68</v>
       </c>
@@ -1894,8 +2014,12 @@
       <c r="K32" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>98</v>
       </c>
@@ -1915,7 +2039,7 @@
         <v>22</v>
       </c>
       <c r="G33" s="3">
-        <f t="shared" ref="G33:G37" si="1">0.9*E33</f>
+        <f t="shared" ref="G33:G37" si="2">0.9*E33</f>
         <v>0.18000000000000002</v>
       </c>
       <c r="H33" s="3"/>
@@ -1927,8 +2051,12 @@
       <c r="K33" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>102</v>
       </c>
@@ -1948,7 +2076,7 @@
         <v>22</v>
       </c>
       <c r="G34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.71</v>
       </c>
       <c r="H34" s="3"/>
@@ -1960,8 +2088,12 @@
       <c r="K34" s="3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>104</v>
       </c>
@@ -1981,7 +2113,7 @@
         <v>22</v>
       </c>
       <c r="G35" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="H35" s="3"/>
@@ -1993,8 +2125,12 @@
       <c r="K35" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>107</v>
       </c>
@@ -2014,7 +2150,7 @@
         <v>22</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3150000</v>
       </c>
       <c r="H36" s="3"/>
@@ -2026,8 +2162,12 @@
       <c r="K36" s="3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>134</v>
       </c>
@@ -2047,8 +2187,8 @@
         <v>22</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" si="1"/>
-        <v>0.87209999999999999</v>
+        <f>1-2*(I37-E37)</f>
+        <v>0.93799999999999994</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="3">
@@ -2058,8 +2198,12 @@
       <c r="K37" s="3" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>111</v>
       </c>
@@ -2089,8 +2233,12 @@
       <c r="K38" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>132</v>
       </c>
@@ -2122,8 +2270,12 @@
       <c r="K39" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>115</v>
       </c>
@@ -2155,8 +2307,12 @@
       <c r="K40" s="3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>117</v>
       </c>
@@ -2188,8 +2344,12 @@
       <c r="K41" s="3" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q41">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>119</v>
       </c>
@@ -2221,8 +2381,12 @@
       <c r="K42" s="3" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>121</v>
       </c>
@@ -2254,8 +2418,12 @@
       <c r="K43" s="3" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>123</v>
       </c>
@@ -2285,8 +2453,12 @@
       <c r="K44" s="3" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q44">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>125</v>
       </c>
@@ -2318,8 +2490,12 @@
       <c r="K45" s="3" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q45">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>135</v>
       </c>
@@ -2349,8 +2525,12 @@
       <c r="K46" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q46">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>128</v>
       </c>
@@ -2383,8 +2563,12 @@
       <c r="K47" s="3" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q47">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>137</v>
       </c>
@@ -2416,8 +2600,12 @@
       <c r="K48" s="3" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q48">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>142</v>
       </c>
@@ -2435,20 +2623,24 @@
         <v>22</v>
       </c>
       <c r="G49" s="3">
-        <f t="shared" ref="G49:G50" si="2">0.9*E49</f>
+        <f t="shared" ref="G49:G50" si="3">0.9*E49</f>
         <v>28.252800000000001</v>
       </c>
       <c r="H49" s="3"/>
       <c r="I49" s="3">
-        <f t="shared" ref="I49:I50" si="3">1.1*E49</f>
+        <f t="shared" ref="I49:I50" si="4">1.1*E49</f>
         <v>34.531200000000005</v>
       </c>
       <c r="J49" s="3"/>
       <c r="K49" s="3" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>143</v>
       </c>
@@ -2466,20 +2658,24 @@
         <v>22</v>
       </c>
       <c r="G50" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>28.390500000000003</v>
       </c>
       <c r="H50" s="3"/>
       <c r="I50" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>34.699500000000008</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q50">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>136</v>
       </c>
@@ -2511,8 +2707,12 @@
       <c r="K51" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>24</v>
       </c>
@@ -2544,8 +2744,12 @@
       <c r="K52" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="Q52">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>58</v>
       </c>
@@ -2576,6 +2780,10 @@
       <c r="J53" s="3"/>
       <c r="K53" s="3" t="s">
         <v>59</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minorly update uncertainty distributions
</commit_message>
<xml_diff>
--- a/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
+++ b/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\biorefineries\TAL\analyses\full\parameter_distributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{734497CB-6070-42A1-B021-9C8F66FDC84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA55DEE3-B1D0-43A5-BA48-041AF17BE2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -540,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -551,6 +551,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -831,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q53"/>
+  <dimension ref="A1:Q94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:XFD37"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2039,7 +2040,7 @@
         <v>22</v>
       </c>
       <c r="G33" s="3">
-        <f t="shared" ref="G33:G37" si="2">0.9*E33</f>
+        <f t="shared" ref="G33:G36" si="2">0.9*E33</f>
         <v>0.18000000000000002</v>
       </c>
       <c r="H33" s="3"/>
@@ -2785,6 +2786,422 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="L63" s="6"/>
+      <c r="M63" s="6"/>
+      <c r="N63" s="6"/>
+      <c r="O63" s="6"/>
+      <c r="P63" s="6"/>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="L64" s="6"/>
+      <c r="M64" s="6"/>
+      <c r="N64" s="6"/>
+      <c r="O64" s="6"/>
+      <c r="P64" s="6"/>
+    </row>
+    <row r="65" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="6"/>
+      <c r="N65" s="6"/>
+      <c r="O65" s="6"/>
+      <c r="P65" s="6"/>
+    </row>
+    <row r="66" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="6"/>
+      <c r="M66" s="6"/>
+      <c r="N66" s="6"/>
+      <c r="O66" s="6"/>
+      <c r="P66" s="6"/>
+    </row>
+    <row r="67" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
+      <c r="L67" s="6"/>
+      <c r="M67" s="6"/>
+      <c r="N67" s="6"/>
+      <c r="O67" s="6"/>
+      <c r="P67" s="6"/>
+    </row>
+    <row r="68" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="L68" s="6"/>
+      <c r="M68" s="6"/>
+      <c r="N68" s="6"/>
+      <c r="O68" s="6"/>
+      <c r="P68" s="6"/>
+    </row>
+    <row r="69" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
+      <c r="L69" s="6"/>
+      <c r="M69" s="6"/>
+      <c r="N69" s="6"/>
+      <c r="O69" s="6"/>
+      <c r="P69" s="6"/>
+    </row>
+    <row r="70" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
+      <c r="J70" s="6"/>
+      <c r="K70" s="6"/>
+      <c r="L70" s="6"/>
+      <c r="M70" s="6"/>
+      <c r="N70" s="6"/>
+      <c r="O70" s="6"/>
+      <c r="P70" s="6"/>
+    </row>
+    <row r="71" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="6"/>
+      <c r="K71" s="6"/>
+      <c r="L71" s="6"/>
+      <c r="M71" s="6"/>
+      <c r="N71" s="6"/>
+      <c r="O71" s="6"/>
+      <c r="P71" s="6"/>
+    </row>
+    <row r="72" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
+      <c r="J72" s="6"/>
+      <c r="K72" s="6"/>
+      <c r="L72" s="6"/>
+      <c r="M72" s="6"/>
+      <c r="N72" s="6"/>
+      <c r="O72" s="6"/>
+      <c r="P72" s="6"/>
+    </row>
+    <row r="73" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="6"/>
+      <c r="K73" s="6"/>
+      <c r="L73" s="6"/>
+      <c r="M73" s="6"/>
+      <c r="N73" s="6"/>
+      <c r="O73" s="6"/>
+      <c r="P73" s="6"/>
+    </row>
+    <row r="74" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="6"/>
+      <c r="M74" s="6"/>
+      <c r="N74" s="6"/>
+      <c r="O74" s="6"/>
+      <c r="P74" s="6"/>
+    </row>
+    <row r="75" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="6"/>
+      <c r="K75" s="6"/>
+      <c r="L75" s="6"/>
+      <c r="M75" s="6"/>
+      <c r="N75" s="6"/>
+      <c r="O75" s="6"/>
+      <c r="P75" s="6"/>
+    </row>
+    <row r="76" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="6"/>
+      <c r="L76" s="6"/>
+      <c r="M76" s="6"/>
+      <c r="N76" s="6"/>
+      <c r="O76" s="6"/>
+      <c r="P76" s="6"/>
+    </row>
+    <row r="77" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="6"/>
+      <c r="M77" s="6"/>
+      <c r="N77" s="6"/>
+      <c r="O77" s="6"/>
+      <c r="P77" s="6"/>
+    </row>
+    <row r="78" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
+      <c r="K78" s="6"/>
+      <c r="L78" s="6"/>
+      <c r="M78" s="6"/>
+      <c r="N78" s="6"/>
+      <c r="O78" s="6"/>
+      <c r="P78" s="6"/>
+    </row>
+    <row r="79" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6"/>
+      <c r="K79" s="6"/>
+      <c r="L79" s="6"/>
+      <c r="M79" s="6"/>
+      <c r="N79" s="6"/>
+      <c r="O79" s="6"/>
+      <c r="P79" s="6"/>
+    </row>
+    <row r="80" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="6"/>
+      <c r="K80" s="6"/>
+      <c r="L80" s="6"/>
+      <c r="M80" s="6"/>
+      <c r="N80" s="6"/>
+      <c r="O80" s="6"/>
+      <c r="P80" s="6"/>
+    </row>
+    <row r="81" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="6"/>
+      <c r="M81" s="6"/>
+      <c r="N81" s="6"/>
+      <c r="O81" s="6"/>
+      <c r="P81" s="6"/>
+    </row>
+    <row r="82" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="6"/>
+      <c r="N82" s="6"/>
+      <c r="O82" s="6"/>
+      <c r="P82" s="6"/>
+    </row>
+    <row r="83" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="L83" s="6"/>
+      <c r="M83" s="6"/>
+      <c r="N83" s="6"/>
+      <c r="O83" s="6"/>
+      <c r="P83" s="6"/>
+    </row>
+    <row r="84" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="6"/>
+      <c r="K84" s="6"/>
+      <c r="L84" s="6"/>
+      <c r="M84" s="6"/>
+      <c r="N84" s="6"/>
+      <c r="O84" s="6"/>
+      <c r="P84" s="6"/>
+    </row>
+    <row r="85" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
+      <c r="L85" s="6"/>
+      <c r="M85" s="6"/>
+      <c r="N85" s="6"/>
+      <c r="O85" s="6"/>
+      <c r="P85" s="6"/>
+    </row>
+    <row r="86" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="6"/>
+      <c r="K86" s="6"/>
+      <c r="L86" s="6"/>
+      <c r="M86" s="6"/>
+      <c r="N86" s="6"/>
+      <c r="O86" s="6"/>
+      <c r="P86" s="6"/>
+    </row>
+    <row r="87" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
+      <c r="K87" s="6"/>
+      <c r="L87" s="6"/>
+      <c r="M87" s="6"/>
+      <c r="N87" s="6"/>
+      <c r="O87" s="6"/>
+      <c r="P87" s="6"/>
+    </row>
+    <row r="88" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6"/>
+      <c r="J88" s="6"/>
+      <c r="K88" s="6"/>
+      <c r="L88" s="6"/>
+      <c r="M88" s="6"/>
+      <c r="N88" s="6"/>
+      <c r="O88" s="6"/>
+      <c r="P88" s="6"/>
+    </row>
+    <row r="89" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="6"/>
+      <c r="J89" s="6"/>
+      <c r="K89" s="6"/>
+      <c r="L89" s="6"/>
+      <c r="M89" s="6"/>
+      <c r="N89" s="6"/>
+      <c r="O89" s="6"/>
+      <c r="P89" s="6"/>
+    </row>
+    <row r="90" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
+      <c r="J90" s="6"/>
+      <c r="K90" s="6"/>
+      <c r="L90" s="6"/>
+      <c r="M90" s="6"/>
+      <c r="N90" s="6"/>
+      <c r="O90" s="6"/>
+      <c r="P90" s="6"/>
+    </row>
+    <row r="91" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="6"/>
+      <c r="K91" s="6"/>
+      <c r="L91" s="6"/>
+      <c r="M91" s="6"/>
+      <c r="N91" s="6"/>
+      <c r="O91" s="6"/>
+      <c r="P91" s="6"/>
+    </row>
+    <row r="92" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+      <c r="J92" s="6"/>
+      <c r="K92" s="6"/>
+      <c r="L92" s="6"/>
+      <c r="M92" s="6"/>
+      <c r="N92" s="6"/>
+      <c r="O92" s="6"/>
+      <c r="P92" s="6"/>
+    </row>
+    <row r="93" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="6"/>
+      <c r="K93" s="6"/>
+      <c r="L93" s="6"/>
+      <c r="M93" s="6"/>
+      <c r="N93" s="6"/>
+      <c r="O93" s="6"/>
+      <c r="P93" s="6"/>
+    </row>
+    <row r="94" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="6"/>
+      <c r="K94" s="6"/>
+      <c r="L94" s="6"/>
+      <c r="M94" s="6"/>
+      <c r="N94" s="6"/>
+      <c r="O94" s="6"/>
+      <c r="P94" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
make bound-capped uncertainty distributions triangular; make sorbate_c,d and sorbate_g,h prod caps same as rest
</commit_message>
<xml_diff>
--- a/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
+++ b/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\biorefineries\TAL\analyses\full\parameter_distributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77983B2-E595-4D24-8FCA-3C59FB6E6217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947A014B-2AF6-4B17-8023-E34C84BD3AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -368,9 +368,6 @@
     <t>R401.P = x</t>
   </si>
   <si>
-    <t>R401.TAL_to_HMTHP_rxn.X = x</t>
-  </si>
-  <si>
     <t>Hydrogenation spent catalyst NiSiO2 replacement rate</t>
   </si>
   <si>
@@ -383,33 +380,15 @@
     <t>R402.mcat_frac = x</t>
   </si>
   <si>
-    <t>Dehydration reaction time</t>
-  </si>
-  <si>
     <t>R402.tau = x</t>
   </si>
   <si>
-    <t>Dehydration temperature</t>
-  </si>
-  <si>
     <t>R402.T = 273.15 + x</t>
   </si>
   <si>
-    <t>Dehydration HMTHP-to-PSA conversion</t>
-  </si>
-  <si>
-    <t>R402.HMTHP_to_PSA_rxn.X = x</t>
-  </si>
-  <si>
-    <t>Dehydration pressure</t>
-  </si>
-  <si>
     <t>R402.P = x</t>
   </si>
   <si>
-    <t>Dehydration spent catalyst Amberlyst70 replacement rate</t>
-  </si>
-  <si>
     <t>R402.spent_catalyst_replacements_per_year  = x</t>
   </si>
   <si>
@@ -434,9 +413,6 @@
     <t>R401.Amberlyst70_catalyst_price = x; fresh_catalyst_Amberlyst70 = x</t>
   </si>
   <si>
-    <t>Dehydration catalyst Amberlyst70:HMTHP ratio</t>
-  </si>
-  <si>
     <t>IPA_fresh.price = x</t>
   </si>
   <si>
@@ -477,6 +453,30 @@
   </si>
   <si>
     <t>KOH_fresh.price = x</t>
+  </si>
+  <si>
+    <t>Etherification &amp; hydrolysis reaction time</t>
+  </si>
+  <si>
+    <t>Etherification &amp; hydrolysis temperature</t>
+  </si>
+  <si>
+    <t>Etherification &amp; hydrolysis pressure</t>
+  </si>
+  <si>
+    <t>Etherification &amp; hydrolysis spent catalyst Amberlyst70 replacement rate</t>
+  </si>
+  <si>
+    <t>R401.TAL_to_HMP_rxn.X = x</t>
+  </si>
+  <si>
+    <t>Etherification &amp; hydrolysis catalyst Amberlyst70:HMP ratio</t>
+  </si>
+  <si>
+    <t>Etherification &amp; hydrolysis HMP-to-PSA conversion</t>
+  </si>
+  <si>
+    <t>R402.HMP_to_PSA_rxn.X = x</t>
   </si>
 </sst>
 </file>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47:H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1214,7 +1214,7 @@
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="Q10">
         <f t="shared" si="0"/>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>7</v>
@@ -1250,7 +1250,7 @@
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -1284,7 +1284,7 @@
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="Q12">
         <f t="shared" si="0"/>
@@ -1321,7 +1321,7 @@
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="Q13">
         <f t="shared" si="0"/>
@@ -1601,7 +1601,7 @@
         <v>0.95</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="G21" s="3">
         <f>0.9*E21</f>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="Q21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
@@ -1964,7 +1964,7 @@
         <v>0.95</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="G31" s="3">
         <f>E31*0.8</f>
@@ -1980,7 +1980,7 @@
       </c>
       <c r="Q31">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
@@ -2207,7 +2207,7 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>99</v>
@@ -2222,19 +2222,22 @@
         <v>0.96899999999999997</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="G38" s="3">
-        <f>1-2*(I38-E38)</f>
-        <v>0.93799999999999994</v>
-      </c>
-      <c r="H38" s="3"/>
+        <f>0.9*E38</f>
+        <v>0.87209999999999999</v>
+      </c>
+      <c r="H38" s="3">
+        <f>E38</f>
+        <v>0.96899999999999997</v>
+      </c>
       <c r="I38" s="3">
         <v>1</v>
       </c>
       <c r="J38" s="3"/>
       <c r="K38" s="3" t="s">
-        <v>110</v>
+        <v>143</v>
       </c>
       <c r="Q38">
         <f t="shared" si="0"/>
@@ -2243,7 +2246,7 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>99</v>
@@ -2252,7 +2255,7 @@
         <v>27</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E39" s="3">
         <v>1</v>
@@ -2269,7 +2272,7 @@
       </c>
       <c r="J39" s="3"/>
       <c r="K39" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q39">
         <f t="shared" si="0"/>
@@ -2278,7 +2281,7 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>99</v>
@@ -2306,7 +2309,7 @@
       </c>
       <c r="J40" s="3"/>
       <c r="K40" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q40">
         <f t="shared" si="0"/>
@@ -2315,7 +2318,7 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>99</v>
@@ -2343,7 +2346,7 @@
       </c>
       <c r="J41" s="3"/>
       <c r="K41" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q41">
         <f t="shared" si="0"/>
@@ -2352,7 +2355,7 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>99</v>
@@ -2380,7 +2383,7 @@
       </c>
       <c r="J42" s="3"/>
       <c r="K42" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="Q42">
         <f t="shared" si="0"/>
@@ -2389,7 +2392,7 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>99</v>
@@ -2417,7 +2420,7 @@
       </c>
       <c r="J43" s="3"/>
       <c r="K43" s="3" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="Q43">
         <f t="shared" si="0"/>
@@ -2426,7 +2429,7 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>99</v>
@@ -2454,7 +2457,7 @@
       </c>
       <c r="J44" s="3"/>
       <c r="K44" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="Q44">
         <f t="shared" si="0"/>
@@ -2463,7 +2466,7 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>99</v>
@@ -2472,7 +2475,7 @@
         <v>27</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E45" s="3">
         <v>1</v>
@@ -2489,7 +2492,7 @@
       </c>
       <c r="J45" s="3"/>
       <c r="K45" s="3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="Q45">
         <f t="shared" si="0"/>
@@ -2498,7 +2501,7 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>99</v>
@@ -2526,7 +2529,7 @@
       </c>
       <c r="J46" s="3"/>
       <c r="K46" s="3" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="Q46">
         <f t="shared" si="0"/>
@@ -2535,7 +2538,7 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>99</v>
@@ -2550,18 +2553,22 @@
         <v>0.999</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="G47" s="3">
-        <v>0.98</v>
-      </c>
-      <c r="H47" s="3"/>
+        <f>0.9*E47</f>
+        <v>0.89910000000000001</v>
+      </c>
+      <c r="H47" s="3">
+        <f>E47</f>
+        <v>0.999</v>
+      </c>
       <c r="I47" s="3">
         <v>1</v>
       </c>
       <c r="J47" s="3"/>
       <c r="K47" s="3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="Q47">
         <f t="shared" si="0"/>
@@ -2570,7 +2577,7 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>99</v>
@@ -2599,7 +2606,7 @@
       </c>
       <c r="J48" s="3"/>
       <c r="K48" s="3" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="Q48">
         <f t="shared" si="0"/>
@@ -2608,7 +2615,7 @@
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>99</v>
@@ -2636,7 +2643,7 @@
       </c>
       <c r="J49" s="3"/>
       <c r="K49" s="3" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="Q49">
         <f t="shared" si="0"/>
@@ -2645,14 +2652,14 @@
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>99</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E50" s="3">
         <v>31.391999999999999</v>
@@ -2671,7 +2678,7 @@
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="Q50">
         <f t="shared" si="0"/>
@@ -2680,14 +2687,14 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>99</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E51" s="3">
         <v>31.545000000000002</v>
@@ -2706,7 +2713,7 @@
       </c>
       <c r="J51" s="3"/>
       <c r="K51" s="3" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="Q51">
         <f t="shared" si="0"/>
@@ -2715,7 +2722,7 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
update reaction time dists
</commit_message>
<xml_diff>
--- a/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
+++ b/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\Spring 2020\BioSTEAM\Bioindustrial-Park\biorefineries\TAL\analyses\full\parameter_distributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FBE7AE-F709-4387-8BA2-DFFB267181C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E355D2A-531F-4050-AB49-E887C4552877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -959,7 +959,7 @@
         <v>79</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q54" si="0">IF(E3=H3, 1, IF(F3=$F$2, 1, 0))</f>
+        <f t="shared" ref="Q3:Q33" si="0">IF(E3=H3, 1, IF(F3=$F$2, 1, 0))</f>
         <v>1</v>
       </c>
     </row>
@@ -2095,10 +2095,6 @@
       <c r="K34" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Q34">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
@@ -2114,27 +2110,23 @@
         <v>15</v>
       </c>
       <c r="E35" s="3">
-        <v>1.9</v>
+        <v>9.4</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G35" s="3">
         <f t="shared" si="2"/>
-        <v>1.71</v>
+        <v>8.4600000000000009</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3">
         <f>1.1*E35</f>
-        <v>2.09</v>
+        <v>10.340000000000002</v>
       </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="Q35">
-        <f t="shared" si="0"/>
-        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
@@ -2169,10 +2161,6 @@
       <c r="K36" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="Q36">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
@@ -2206,10 +2194,6 @@
       <c r="K37" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="Q37">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
@@ -2246,7 +2230,7 @@
         <v>143</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q38" si="3">IF(E38=H38, 1, IF(F38=$F$2, 1, 0))</f>
         <v>1</v>
       </c>
     </row>
@@ -2279,10 +2263,6 @@
       <c r="J39" s="3"/>
       <c r="K39" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="Q39">
-        <f t="shared" si="0"/>
-        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
@@ -2317,10 +2297,6 @@
       <c r="K40" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="Q40">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
@@ -2336,27 +2312,23 @@
         <v>15</v>
       </c>
       <c r="E41" s="3">
-        <v>3.1</v>
+        <v>6.1</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G41" s="3">
         <f>0.9*E41</f>
-        <v>2.79</v>
+        <v>5.49</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="3">
         <f>1.1*E41</f>
-        <v>3.4100000000000006</v>
+        <v>6.71</v>
       </c>
       <c r="J41" s="3"/>
       <c r="K41" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="Q41">
-        <f t="shared" si="0"/>
-        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
@@ -2391,10 +2363,6 @@
       <c r="K42" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="Q42">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
@@ -2428,10 +2396,6 @@
       <c r="K43" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="Q43">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
@@ -2465,10 +2429,6 @@
       <c r="K44" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="Q44">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
@@ -2500,10 +2460,6 @@
       <c r="K45" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="Q45">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
@@ -2519,28 +2475,24 @@
         <v>15</v>
       </c>
       <c r="E46" s="3">
-        <v>9.51</v>
+        <v>19</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G46" s="3">
         <f>0.9*E46</f>
-        <v>8.5589999999999993</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="3">
         <f>1.1*E46</f>
-        <v>10.461</v>
+        <v>20.900000000000002</v>
       </c>
       <c r="J46" s="3"/>
       <c r="K46" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="Q46">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
@@ -2575,10 +2527,6 @@
       <c r="J47" s="3"/>
       <c r="K47" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="Q47">
-        <f t="shared" si="0"/>
-        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
@@ -2614,12 +2562,8 @@
       <c r="K48" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="Q48">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>129</v>
       </c>
@@ -2651,12 +2595,8 @@
       <c r="K49" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="Q49">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>134</v>
       </c>
@@ -2674,24 +2614,20 @@
         <v>22</v>
       </c>
       <c r="G50" s="3">
-        <f t="shared" ref="G50:G51" si="3">0.9*E50</f>
+        <f t="shared" ref="G50:G51" si="4">0.9*E50</f>
         <v>28.252800000000001</v>
       </c>
       <c r="H50" s="3"/>
       <c r="I50" s="3">
-        <f t="shared" ref="I50:I51" si="4">1.1*E50</f>
+        <f t="shared" ref="I50:I51" si="5">1.1*E50</f>
         <v>34.531200000000005</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="Q50">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>135</v>
       </c>
@@ -2709,24 +2645,20 @@
         <v>22</v>
       </c>
       <c r="G51" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>28.390500000000003</v>
       </c>
       <c r="H51" s="3"/>
       <c r="I51" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>34.699500000000008</v>
       </c>
       <c r="J51" s="3"/>
       <c r="K51" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="Q51">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>128</v>
       </c>
@@ -2758,12 +2690,8 @@
       <c r="K52" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="Q52">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>24</v>
       </c>
@@ -2795,12 +2723,8 @@
       <c r="K53" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="Q53">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>58</v>
       </c>
@@ -2831,10 +2755,6 @@
       <c r="J54" s="3"/>
       <c r="K54" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="Q54">
-        <f t="shared" si="0"/>
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update feedstock capacities for FGI
</commit_message>
<xml_diff>
--- a/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
+++ b/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_Sorbate_A.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\repository_clones\Bioindustrial-Park\biorefineries\TAL\analyses\full\parameter_distributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE48D0E5-B75F-473D-9201-6CBB76F6BD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E016F95-53DC-4359-B653-6E6C7CF572A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="1740" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="146">
   <si>
     <t>Parameter name</t>
   </si>
@@ -288,9 +288,6 @@
   </si>
   <si>
     <t>tea.income_tax = x</t>
-  </si>
-  <si>
-    <t>Cortes-Pena et al. 2023; Huang et al. 2016</t>
   </si>
   <si>
     <t>TAL solubility multiplier</t>
@@ -511,12 +508,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -546,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -557,6 +560,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -885,7 +890,7 @@
         <v>38</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
@@ -923,80 +928,81 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="6">
         <v>180</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="6">
         <v>120</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="6">
         <f>E3</f>
         <v>180</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="6">
         <v>240</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K3" s="3" t="s">
+      <c r="J3" s="6"/>
+      <c r="K3" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="7">
         <f>IF(E3=H3, 1, IF(F3=$F$2, 1, 0))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="3">
-        <v>3.4500000000000003E-2</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="6">
+        <v>3.5920000000000001E-2</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="3">
-        <v>2.76E-2</v>
-      </c>
-      <c r="H4" s="3">
-        <v>3.4500000000000003E-2</v>
-      </c>
-      <c r="I4" s="3">
-        <v>4.1399999999999999E-2</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3" t="s">
+      <c r="G4" s="6">
+        <f>E4*0.8</f>
+        <v>2.8736000000000001E-2</v>
+      </c>
+      <c r="H4" s="6">
+        <f>E4</f>
+        <v>3.5920000000000001E-2</v>
+      </c>
+      <c r="I4" s="6">
+        <f>E4*1.2</f>
+        <v>4.3103999999999996E-2</v>
+      </c>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="Q4">
-        <f t="shared" ref="Q4:Q33" si="0">IF(E4=H4, 1, IF(F4=$F$2, 1, 0))</f>
+      <c r="Q4" s="7">
+        <f t="shared" ref="Q4" si="0">IF(E4=H4, 1, IF(F4=$F$2, 1, 0))</f>
         <v>1</v>
       </c>
     </row>
@@ -1033,7 +1039,7 @@
         <v>56</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q4:Q33" si="1">IF(E5=H5, 1, IF(F5=$F$2, 1, 0))</f>
         <v>1</v>
       </c>
     </row>
@@ -1070,7 +1076,7 @@
         <v>36</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1110,7 +1116,7 @@
         <v>51</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1147,13 +1153,13 @@
         <v>52</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>7</v>
@@ -1179,16 +1185,16 @@
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>7</v>
@@ -1214,16 +1220,16 @@
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>7</v>
@@ -1250,16 +1256,16 @@
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>7</v>
@@ -1280,7 +1286,7 @@
         <v>5</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" ref="H12" si="1">E12</f>
+        <f t="shared" ref="H12" si="2">E12</f>
         <v>33</v>
       </c>
       <c r="I12" s="3">
@@ -1288,16 +1294,16 @@
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>7</v>
@@ -1325,10 +1331,10 @@
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1368,7 +1374,7 @@
         <v>59</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1403,7 +1409,7 @@
         <v>83</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1438,7 +1444,7 @@
         <v>82</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1475,13 +1481,13 @@
         <v>32</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>44</v>
@@ -1509,10 +1515,10 @@
         <v>76</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1527,7 +1533,7 @@
         <v>27</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E19" s="3">
         <v>10</v>
@@ -1549,13 +1555,13 @@
         <v>45</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>44</v>
@@ -1581,10 +1587,10 @@
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1620,7 +1626,7 @@
         <v>33</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1657,7 +1663,7 @@
         <v>40</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1694,7 +1700,7 @@
         <v>63</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1731,7 +1737,7 @@
         <v>34</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1768,7 +1774,7 @@
         <v>35</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1805,7 +1811,7 @@
         <v>74</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1842,7 +1848,7 @@
         <v>75</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1877,13 +1883,13 @@
         <v>70</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>54</v>
@@ -1909,10 +1915,10 @@
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1947,7 +1953,7 @@
         <v>55</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1983,7 +1989,7 @@
         <v>72</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2020,7 +2026,7 @@
         <v>66</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2057,22 +2063,22 @@
         <v>68</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="E34" s="3">
         <v>0.2</v>
@@ -2081,7 +2087,7 @@
         <v>22</v>
       </c>
       <c r="G34" s="3">
-        <f t="shared" ref="G34:G37" si="2">0.9*E34</f>
+        <f t="shared" ref="G34:G37" si="3">0.9*E34</f>
         <v>0.18000000000000002</v>
       </c>
       <c r="H34" s="3"/>
@@ -2091,7 +2097,7 @@
       </c>
       <c r="J34" s="3"/>
       <c r="K34" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q34">
         <f>IF(E34=H34, 1, IF(F34=$F$2, 1, 0))</f>
@@ -2100,10 +2106,10 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>27</v>
@@ -2118,7 +2124,7 @@
         <v>22</v>
       </c>
       <c r="G35" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.4600000000000009</v>
       </c>
       <c r="H35" s="3"/>
@@ -2128,7 +2134,7 @@
       </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q35">
         <f>IF(E35=H35, 1, IF(F35=$F$2, 1, 0))</f>
@@ -2137,16 +2143,16 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="E36" s="3">
         <v>100</v>
@@ -2155,7 +2161,7 @@
         <v>22</v>
       </c>
       <c r="G36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>90</v>
       </c>
       <c r="H36" s="3"/>
@@ -2165,25 +2171,25 @@
       </c>
       <c r="J36" s="3"/>
       <c r="K36" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q36">
-        <f t="shared" ref="Q36:Q54" si="3">IF(E36=H36, 1, IF(F36=$F$2, 1, 0))</f>
+        <f t="shared" ref="Q36:Q54" si="4">IF(E36=H36, 1, IF(F36=$F$2, 1, 0))</f>
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E37" s="3">
         <v>3500000</v>
@@ -2192,7 +2198,7 @@
         <v>22</v>
       </c>
       <c r="G37" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3150000</v>
       </c>
       <c r="H37" s="3"/>
@@ -2202,19 +2208,19 @@
       </c>
       <c r="J37" s="3"/>
       <c r="K37" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>27</v>
@@ -2238,25 +2244,25 @@
       </c>
       <c r="J38" s="3"/>
       <c r="K38" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>110</v>
       </c>
       <c r="E39" s="3">
         <v>1</v>
@@ -2273,25 +2279,25 @@
       </c>
       <c r="J39" s="3"/>
       <c r="K39" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="E40" s="3">
         <v>0.5</v>
@@ -2310,19 +2316,19 @@
       </c>
       <c r="J40" s="3"/>
       <c r="K40" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>27</v>
@@ -2347,25 +2353,25 @@
       </c>
       <c r="J41" s="3"/>
       <c r="K41" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E42" s="3">
         <v>160</v>
@@ -2384,19 +2390,19 @@
       </c>
       <c r="J42" s="3"/>
       <c r="K42" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>27</v>
@@ -2421,25 +2427,25 @@
       </c>
       <c r="J43" s="3"/>
       <c r="K43" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="Q43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E44" s="3">
         <v>2000000</v>
@@ -2458,25 +2464,25 @@
       </c>
       <c r="J44" s="3"/>
       <c r="K44" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E45" s="3">
         <v>1</v>
@@ -2493,19 +2499,19 @@
       </c>
       <c r="J45" s="3"/>
       <c r="K45" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>27</v>
@@ -2530,19 +2536,19 @@
       </c>
       <c r="J46" s="3"/>
       <c r="K46" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>27</v>
@@ -2565,25 +2571,25 @@
       </c>
       <c r="J47" s="3"/>
       <c r="K47" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E48" s="3">
         <f>130</f>
@@ -2603,25 +2609,25 @@
       </c>
       <c r="J48" s="3"/>
       <c r="K48" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E49" s="3">
         <v>2000000</v>
@@ -2640,23 +2646,23 @@
       </c>
       <c r="J49" s="3"/>
       <c r="K49" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Q49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E50" s="3">
         <v>31.391999999999999</v>
@@ -2665,33 +2671,33 @@
         <v>22</v>
       </c>
       <c r="G50" s="3">
-        <f t="shared" ref="G50:G51" si="4">0.9*E50</f>
+        <f t="shared" ref="G50:G51" si="5">0.9*E50</f>
         <v>28.252800000000001</v>
       </c>
       <c r="H50" s="3"/>
       <c r="I50" s="3">
-        <f t="shared" ref="I50:I51" si="5">1.1*E50</f>
+        <f t="shared" ref="I50:I51" si="6">1.1*E50</f>
         <v>34.531200000000005</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E51" s="3">
         <v>31.545000000000002</v>
@@ -2700,26 +2706,26 @@
         <v>22</v>
       </c>
       <c r="G51" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>28.390500000000003</v>
       </c>
       <c r="H51" s="3"/>
       <c r="I51" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>34.699500000000008</v>
       </c>
       <c r="J51" s="3"/>
       <c r="K51" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>14</v>
@@ -2750,7 +2756,7 @@
         <v>62</v>
       </c>
       <c r="Q52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2787,7 +2793,7 @@
         <v>37</v>
       </c>
       <c r="Q53">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2824,7 +2830,7 @@
         <v>58</v>
       </c>
       <c r="Q54">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>